<commit_message>
fix: fixed stocks being columns instead of rows
Before the stock names would be columns, but it made more sense for them to be rows that could e.g. be filtered in a database
</commit_message>
<xml_diff>
--- a/samples/sample.xlsx
+++ b/samples/sample.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,345 +436,393 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>Day's Range</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>SCHB</t>
+          <t>PE Ratio (TTM)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>NKE</t>
+          <t>YTD Daily Total Return</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Net Assets</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Beta (5Y Monthly)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Bid</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>52 Week Range</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Volume</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Yield</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Volume</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Previous Close</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Ask</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Earnings Date</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Forward Dividend &amp; Yield</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>EPS (TTM)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>PE Ratio (TTM)</t>
+          <t>SCHB</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>17.92</t>
+          <t>52.88 - 53.12</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>21.72</t>
+          <t>52.89</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>33.80</t>
-        </is>
-      </c>
+          <t>18.99%</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>53.12</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>23B</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.01</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>52.76 x 1800</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>40.92 - 53.43</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>694,175</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1.47%</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>738,364</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>52.92</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>53.88 x 4000</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Open</t>
+          <t>GOOGL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>172.17</t>
+          <t>118.73 - 120.99</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>53.12</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>108.00</t>
+          <t>1.05</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>120.62</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>120.06 x 900</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>83.34 - 129.04</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>33,916,937</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>68,300,790</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>119.20</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>120.09 x 800</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Jul 25, 2023</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>1.526T</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>N/A (N/A)</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>4.40</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Ask</t>
+          <t>NKE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>171.30 x 800</t>
+          <t>107.51 - 109.29</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>53.08 x 2200</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>108.95 x 1800</t>
+          <t>1.12</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>108.00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>109.06 x 1300</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>82.22 - 131.31</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>8,096,234</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>6,617,479</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>107.53</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>109.06 x 1100</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Sep 27, 2023 - Oct 02, 2023</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>167.624B</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>1.36 (1.26%)</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3.23</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>52 Week Range</t>
+          <t>AXL</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>130.65 - 182.15</t>
+          <t>9.14 - 9.41</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>40.92 - 53.43</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>82.22 - 131.31</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Market Cap</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>126.908B</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>167.778B</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Forward Dividend &amp; Yield</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2.40 (1.36%)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1.36 (1.26%)</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Volume</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2,847,747</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>694,175</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>8,096,234</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Earnings Date</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Jul 21, 2023</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Sep 27, 2023 - Oct 02, 2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Day's Range</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>167.42 - 173.34</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>52.88 - 53.12</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>107.54 - 109.29</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Volume</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Jul 06, 2023</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>0.03%</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Jun 02, 2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>EPS (TTM)</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>9.53</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>3.23</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Previous Close</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>177.11</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>52.92</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>107.53</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Bid</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>171.13 x 1000</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>53.07 x 900</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>108.93 x 1200</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Net Assets</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>23B</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Beta (5Y Monthly)</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1.01</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>YTD Daily Total Return</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>18.99%</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Yield</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>1.47%</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>9.31</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>9.15 x 900</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>6.61 - 11.96</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>1,196,275</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>1,448,198</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>9.18</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>9.40 x 3100</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Aug 04, 2023</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>1.075B</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>N/A (N/A)</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>0.49</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>